<commit_message>
Updated margin data spreadsheet
</commit_message>
<xml_diff>
--- a/MarginData.xlsx
+++ b/MarginData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rainy\Documents\GitHub\Economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD27C7F-E220-4258-B3F5-F685589DD404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F8C65B-536E-41B6-90F0-54975341CE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30938" yWindow="2730" windowWidth="21600" windowHeight="11542" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MarginData" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="11">
   <si>
     <t>Margin Debt</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>Stitched Free Credit Balances in Customers' Securities Margin Accounts</t>
-  </si>
-  <si>
-    <t>11/31/2021</t>
   </si>
 </sst>
 </file>
@@ -581,7 +578,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -604,9 +601,6 @@
     </xf>
     <xf numFmtId="3" fontId="20" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -931,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J767"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1365,8 +1359,8 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
-        <v>11</v>
+      <c r="A13" s="2">
+        <v>44530</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>3</v>

</xml_diff>